<commit_message>
cleaning up excel file
</commit_message>
<xml_diff>
--- a/revenue-streamlit/tenancy_list_scenario_01.xlsx
+++ b/revenue-streamlit/tenancy_list_scenario_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mawan/Development/office/revenue-streamlit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F0D6FD-DF16-7D4F-A0AA-FE3AB5EB63D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF30AED2-E57C-7043-BA86-0ECE30EDDDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22660" yWindow="9000" windowWidth="22660" windowHeight="14380" tabRatio="765" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" tabRatio="765" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="2" r:id="rId1"/>
@@ -1274,7 +1274,7 @@
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1503,9 +1503,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -2563,13 +2560,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>246807</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>132619</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>288616</xdr:colOff>
-      <xdr:row>165</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>77683</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2641,13 +2638,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>234894</xdr:colOff>
-      <xdr:row>166</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>86989</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>276703</xdr:colOff>
-      <xdr:row>179</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>32053</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2719,13 +2716,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>222981</xdr:colOff>
-      <xdr:row>179</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>131271</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>264790</xdr:colOff>
-      <xdr:row>200</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>157345</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2836,21 +2833,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A0023E2-6AF7-7B4C-AA3C-5526EA8C01E9}" name="Table1" displayName="Table1" ref="A1:N160" totalsRowCount="1" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
-  <autoFilter ref="A1:N159" xr:uid="{1A0023E2-6AF7-7B4C-AA3C-5526EA8C01E9}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="25"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Office"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:N96">
-    <sortCondition ref="J1:J159"/>
-  </sortState>
+  <autoFilter ref="A1:N159" xr:uid="{1A0023E2-6AF7-7B4C-AA3C-5526EA8C01E9}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{82702CBB-B7D8-5C45-8EE8-39144A9E6839}" name="No" totalsRowLabel="Total" dataDxfId="27" totalsRowDxfId="13"/>
     <tableColumn id="13" xr3:uid="{81693DE1-7410-4E03-8801-E72BA5AA4D0C}" name="Location" dataDxfId="26" totalsRowDxfId="12"/>
@@ -3246,7 +3229,8 @@
   <dimension ref="A1:N160"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="93" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H166" sqref="H166"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3308,7 +3292,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="29">
         <v>1</v>
       </c>
@@ -3350,7 +3334,7 @@
       </c>
       <c r="N2" s="20"/>
     </row>
-    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="29">
         <v>2</v>
       </c>
@@ -3385,7 +3369,7 @@
         <v>49125</v>
       </c>
       <c r="L3" s="6">
-        <f t="shared" ref="L3:L13" si="0">362500*11.5/12</f>
+        <f>362500*11.5/12</f>
         <v>347395.83333333331</v>
       </c>
       <c r="M3" s="6">
@@ -3393,7 +3377,7 @@
       </c>
       <c r="N3" s="20"/>
     </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="29">
         <v>3</v>
       </c>
@@ -3428,7 +3412,7 @@
         <v>49125</v>
       </c>
       <c r="L4" s="6">
-        <f t="shared" si="0"/>
+        <f>362500*11.5/12</f>
         <v>347395.83333333331</v>
       </c>
       <c r="M4" s="6">
@@ -3436,7 +3420,7 @@
       </c>
       <c r="N4" s="20"/>
     </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="29">
         <v>4</v>
       </c>
@@ -3471,7 +3455,7 @@
         <v>49125</v>
       </c>
       <c r="L5" s="6">
-        <f t="shared" si="0"/>
+        <f>362500*11.5/12</f>
         <v>347395.83333333331</v>
       </c>
       <c r="M5" s="6">
@@ -3479,7 +3463,7 @@
       </c>
       <c r="N5" s="20"/>
     </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="29">
         <v>5</v>
       </c>
@@ -3512,7 +3496,7 @@
         <v>49125</v>
       </c>
       <c r="L6" s="6">
-        <f t="shared" si="0"/>
+        <f>362500*11.5/12</f>
         <v>347395.83333333331</v>
       </c>
       <c r="M6" s="6">
@@ -3520,7 +3504,7 @@
       </c>
       <c r="N6" s="20"/>
     </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="29">
         <v>6</v>
       </c>
@@ -3555,7 +3539,7 @@
         <v>49125</v>
       </c>
       <c r="L7" s="6">
-        <f t="shared" si="0"/>
+        <f>362500*11.5/12</f>
         <v>347395.83333333331</v>
       </c>
       <c r="M7" s="6">
@@ -3563,7 +3547,7 @@
       </c>
       <c r="N7" s="20"/>
     </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="29">
         <v>7</v>
       </c>
@@ -3598,7 +3582,7 @@
         <v>49125</v>
       </c>
       <c r="L8" s="6">
-        <f t="shared" si="0"/>
+        <f>362500*11.5/12</f>
         <v>347395.83333333331</v>
       </c>
       <c r="M8" s="6">
@@ -3606,7 +3590,7 @@
       </c>
       <c r="N8" s="20"/>
     </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="29">
         <v>8</v>
       </c>
@@ -3641,7 +3625,7 @@
         <v>49125</v>
       </c>
       <c r="L9" s="6">
-        <f t="shared" si="0"/>
+        <f>362500*11.5/12</f>
         <v>347395.83333333331</v>
       </c>
       <c r="M9" s="6">
@@ -3649,7 +3633,7 @@
       </c>
       <c r="N9" s="20"/>
     </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="29">
         <v>9</v>
       </c>
@@ -3684,7 +3668,7 @@
         <v>49125</v>
       </c>
       <c r="L10" s="6">
-        <f t="shared" si="0"/>
+        <f>362500*11.5/12</f>
         <v>347395.83333333331</v>
       </c>
       <c r="M10" s="6">
@@ -3692,7 +3676,7 @@
       </c>
       <c r="N10" s="20"/>
     </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="29">
         <v>10</v>
       </c>
@@ -3727,7 +3711,7 @@
         <v>49125</v>
       </c>
       <c r="L11" s="6">
-        <f t="shared" si="0"/>
+        <f>362500*11.5/12</f>
         <v>347395.83333333331</v>
       </c>
       <c r="M11" s="6">
@@ -3735,7 +3719,7 @@
       </c>
       <c r="N11" s="20"/>
     </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="29">
         <v>11</v>
       </c>
@@ -3770,7 +3754,7 @@
         <v>49125</v>
       </c>
       <c r="L12" s="6">
-        <f t="shared" si="0"/>
+        <f>362500*11.5/12</f>
         <v>347395.83333333331</v>
       </c>
       <c r="M12" s="6">
@@ -3778,7 +3762,7 @@
       </c>
       <c r="N12" s="20"/>
     </row>
-    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="29">
         <v>12</v>
       </c>
@@ -3813,7 +3797,7 @@
         <v>49125</v>
       </c>
       <c r="L13" s="6">
-        <f t="shared" si="0"/>
+        <f>362500*11.5/12</f>
         <v>347395.83333333331</v>
       </c>
       <c r="M13" s="6">
@@ -3821,9 +3805,9 @@
       </c>
       <c r="N13" s="20"/>
     </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="29">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>175</v>
@@ -3832,19 +3816,19 @@
         <v>33</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>173</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>182</v>
+        <v>129</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="35">
-        <v>704.51</v>
+        <v>22</v>
+      </c>
+      <c r="H14" s="8">
+        <v>925.4</v>
       </c>
       <c r="I14" s="32" t="s">
         <v>3</v>
@@ -3853,19 +3837,20 @@
         <v>43647</v>
       </c>
       <c r="K14" s="5">
-        <v>44773</v>
+        <v>49125</v>
       </c>
       <c r="L14" s="6">
-        <v>450000</v>
+        <f>362500*11.5/12</f>
+        <v>347395.83333333331</v>
       </c>
       <c r="M14" s="6">
-        <v>70000</v>
+        <v>84100</v>
       </c>
       <c r="N14" s="20"/>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="29">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>175</v>
@@ -3880,10 +3865,10 @@
         <v>173</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>121</v>
+        <v>25</v>
       </c>
       <c r="H15" s="35">
         <v>704.51</v>
@@ -3892,22 +3877,22 @@
         <v>3</v>
       </c>
       <c r="J15" s="7">
-        <v>44774</v>
+        <v>43647</v>
       </c>
       <c r="K15" s="5">
-        <v>49156</v>
+        <v>44773</v>
       </c>
       <c r="L15" s="6">
-        <v>383000</v>
+        <v>450000</v>
       </c>
       <c r="M15" s="6">
         <v>70000</v>
       </c>
       <c r="N15" s="20"/>
     </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="29">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>175</v>
@@ -3916,7 +3901,7 @@
         <v>33</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>173</v>
@@ -3925,120 +3910,119 @@
         <v>129</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="8">
-        <v>925.4</v>
+        <v>121</v>
+      </c>
+      <c r="H16" s="35">
+        <v>704.51</v>
       </c>
       <c r="I16" s="32" t="s">
         <v>3</v>
       </c>
       <c r="J16" s="7">
-        <v>43647</v>
+        <v>44774</v>
       </c>
       <c r="K16" s="5">
-        <v>49125</v>
+        <v>49156</v>
       </c>
       <c r="L16" s="6">
-        <f>362500*11.5/12</f>
-        <v>347395.83333333331</v>
+        <v>383000</v>
       </c>
       <c r="M16" s="6">
-        <v>84100</v>
+        <v>70000</v>
       </c>
       <c r="N16" s="20"/>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="29">
+        <v>16</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" s="2">
+        <v>32</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="H17" s="38">
+        <v>357.73</v>
+      </c>
+      <c r="I17" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="7">
+        <v>42826</v>
+      </c>
+      <c r="K17" s="5">
+        <v>49034</v>
+      </c>
+      <c r="L17" s="6">
+        <v>383000</v>
+      </c>
+      <c r="M17" s="6">
+        <v>70000</v>
+      </c>
+      <c r="N17" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="29">
+        <v>17</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="4">
+        <v>32</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="8">
+        <v>440.41</v>
+      </c>
+      <c r="I18" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="39">
+        <v>44484</v>
+      </c>
+      <c r="K18" s="5">
+        <v>49292</v>
+      </c>
+      <c r="L18" s="40">
+        <v>490000</v>
+      </c>
+      <c r="M18" s="40">
+        <v>70000</v>
+      </c>
+      <c r="N18" s="20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="29">
         <v>18</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="C17" s="4">
-        <v>32</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="H17" s="36">
-        <v>347.01</v>
-      </c>
-      <c r="I17" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="J17" s="37">
-        <v>44927</v>
-      </c>
-      <c r="K17" s="37">
-        <v>49125</v>
-      </c>
-      <c r="L17" s="14">
-        <v>347396</v>
-      </c>
-      <c r="M17" s="14">
-        <v>84100</v>
-      </c>
-      <c r="N17" s="20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="29">
-        <v>16</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="C18" s="2">
-        <v>32</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H18" s="38">
-        <v>357.73</v>
-      </c>
-      <c r="I18" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="J18" s="7">
-        <v>42826</v>
-      </c>
-      <c r="K18" s="5">
-        <v>49034</v>
-      </c>
-      <c r="L18" s="6">
-        <v>383000</v>
-      </c>
-      <c r="M18" s="6">
-        <v>70000</v>
-      </c>
-      <c r="N18" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="29">
-        <v>17</v>
       </c>
       <c r="B19" s="29" t="s">
         <v>175</v>
@@ -4046,8 +4030,8 @@
       <c r="C19" s="4">
         <v>32</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>180</v>
+      <c r="D19" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>173</v>
@@ -4056,32 +4040,34 @@
         <v>182</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H19" s="8">
-        <v>440.41</v>
+        <v>185</v>
+      </c>
+      <c r="H19" s="36">
+        <v>347.01</v>
       </c>
       <c r="I19" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J19" s="39">
-        <v>44484</v>
-      </c>
-      <c r="K19" s="5">
-        <v>49292</v>
-      </c>
-      <c r="L19" s="40">
-        <v>490000</v>
-      </c>
-      <c r="M19" s="40">
-        <v>70000</v>
+      <c r="J19" s="37">
+        <v>44927</v>
+      </c>
+      <c r="K19" s="37">
+        <v>49125</v>
+      </c>
+      <c r="L19" s="14">
+        <v>347396</v>
+      </c>
+      <c r="M19" s="14">
+        <v>84100</v>
       </c>
       <c r="N19" s="20" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="29"/>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="29">
+        <v>19</v>
+      </c>
       <c r="B20" s="29" t="s">
         <v>175</v>
       </c>
@@ -4089,7 +4075,7 @@
         <v>32</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>180</v>
+        <v>8</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>173</v>
@@ -4098,23 +4084,29 @@
         <v>182</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>56</v>
+        <v>185</v>
       </c>
       <c r="H20" s="8">
-        <v>440.41</v>
+        <v>488.65</v>
       </c>
       <c r="I20" s="32" t="s">
         <v>3</v>
       </c>
       <c r="J20" s="39">
-        <v>49310</v>
-      </c>
-      <c r="K20" s="5"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
+        <v>44927</v>
+      </c>
+      <c r="K20" s="5">
+        <v>49125</v>
+      </c>
+      <c r="L20" s="6">
+        <v>347396</v>
+      </c>
+      <c r="M20" s="40">
+        <v>84100</v>
+      </c>
       <c r="N20" s="20"/>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="29">
         <v>20</v>
       </c>
@@ -4125,7 +4117,7 @@
         <v>32</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>8</v>
+        <v>180</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>173</v>
@@ -4134,40 +4126,34 @@
         <v>182</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>185</v>
+        <v>56</v>
       </c>
       <c r="H21" s="8">
-        <v>488.65</v>
+        <v>440.41</v>
       </c>
       <c r="I21" s="32" t="s">
         <v>3</v>
       </c>
       <c r="J21" s="39">
-        <v>44927</v>
-      </c>
-      <c r="K21" s="5">
-        <v>49125</v>
-      </c>
-      <c r="L21" s="6">
-        <v>347396</v>
-      </c>
-      <c r="M21" s="40">
-        <v>84100</v>
-      </c>
+        <v>49310</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
       <c r="N21" s="20"/>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="29">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="4">
         <v>31</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>24</v>
+      <c r="D22" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>173</v>
@@ -4176,40 +4162,40 @@
         <v>129</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="H22" s="8">
-        <v>704.57</v>
+        <v>1623.88</v>
       </c>
       <c r="I22" s="32" t="s">
         <v>3</v>
       </c>
       <c r="J22" s="7">
-        <v>43556</v>
+        <v>45108</v>
       </c>
       <c r="K22" s="5">
-        <v>44926</v>
+        <v>49125</v>
       </c>
       <c r="L22" s="6">
-        <v>367500</v>
+        <v>347396</v>
       </c>
       <c r="M22" s="6">
-        <v>70000</v>
+        <v>84100</v>
       </c>
       <c r="N22" s="20"/>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="29">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="29" t="s">
         <v>175</v>
       </c>
       <c r="C23" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>173</v>
@@ -4218,31 +4204,31 @@
         <v>129</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>192</v>
+        <v>29</v>
       </c>
       <c r="H23" s="8">
-        <v>162.18</v>
+        <v>704.57</v>
       </c>
       <c r="I23" s="32" t="s">
         <v>3</v>
       </c>
       <c r="J23" s="7">
-        <v>44927</v>
+        <v>43556</v>
       </c>
       <c r="K23" s="5">
-        <v>49309</v>
+        <v>44926</v>
       </c>
       <c r="L23" s="6">
-        <v>383000</v>
+        <v>367500</v>
       </c>
       <c r="M23" s="6">
         <v>70000</v>
       </c>
       <c r="N23" s="20"/>
     </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="29">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="29" t="s">
         <v>175</v>
@@ -4251,7 +4237,7 @@
         <v>30</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>173</v>
@@ -4263,7 +4249,7 @@
         <v>192</v>
       </c>
       <c r="H24" s="8">
-        <v>168.21</v>
+        <v>162.18</v>
       </c>
       <c r="I24" s="32" t="s">
         <v>3</v>
@@ -4282,9 +4268,9 @@
       </c>
       <c r="N24" s="20"/>
     </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="29">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="29" t="s">
         <v>175</v>
@@ -4293,7 +4279,7 @@
         <v>30</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>173</v>
@@ -4302,19 +4288,19 @@
         <v>129</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>30</v>
+        <v>192</v>
       </c>
       <c r="H25" s="8">
-        <v>453.45</v>
+        <v>168.21</v>
       </c>
       <c r="I25" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J25" s="41">
-        <v>43709</v>
+      <c r="J25" s="7">
+        <v>44927</v>
       </c>
       <c r="K25" s="5">
-        <v>49187</v>
+        <v>49309</v>
       </c>
       <c r="L25" s="6">
         <v>383000</v>
@@ -4324,43 +4310,49 @@
       </c>
       <c r="N25" s="20"/>
     </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="29">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B26" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="C26" s="4">
-        <v>27</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>36</v>
+      <c r="C26" s="2">
+        <v>30</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>173</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>182</v>
+        <v>129</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="H26" s="8">
-        <v>1116.77</v>
+        <v>453.45</v>
       </c>
       <c r="I26" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="7">
-        <v>44927</v>
-      </c>
-      <c r="K26" s="5"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
+      <c r="J26" s="41">
+        <v>43709</v>
+      </c>
+      <c r="K26" s="5">
+        <v>49187</v>
+      </c>
+      <c r="L26" s="6">
+        <v>383000</v>
+      </c>
+      <c r="M26" s="6">
+        <v>70000</v>
+      </c>
       <c r="N26" s="20"/>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="29">
         <v>26</v>
       </c>
@@ -4400,7 +4392,7 @@
       </c>
       <c r="N27" s="20"/>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="29">
         <v>27</v>
       </c>
@@ -4442,7 +4434,7 @@
       </c>
       <c r="N28" s="20"/>
     </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="29">
         <v>28</v>
       </c>
@@ -4485,7 +4477,7 @@
       </c>
       <c r="N29" s="20"/>
     </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="29">
         <v>29</v>
       </c>
@@ -4527,7 +4519,7 @@
       </c>
       <c r="N30" s="20"/>
     </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="29">
         <v>30</v>
       </c>
@@ -4563,7 +4555,7 @@
       <c r="M31" s="6"/>
       <c r="N31" s="20"/>
     </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="29">
         <v>31</v>
       </c>
@@ -4605,7 +4597,7 @@
       </c>
       <c r="N32" s="20"/>
     </row>
-    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="29">
         <v>32</v>
       </c>
@@ -4647,72 +4639,72 @@
       </c>
       <c r="N33" s="20"/>
     </row>
-    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="29">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B34" s="29" t="s">
         <v>175</v>
       </c>
       <c r="C34" s="4">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>173</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H34" s="36">
-        <v>306.92</v>
+        <v>37</v>
+      </c>
+      <c r="H34" s="8">
+        <v>1179.0999999999999</v>
       </c>
       <c r="I34" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J34" s="39">
-        <v>44927</v>
+      <c r="J34" s="7">
+        <v>43647</v>
       </c>
       <c r="K34" s="5">
-        <v>49155</v>
-      </c>
-      <c r="L34" s="40">
-        <v>367500</v>
-      </c>
-      <c r="M34" s="40">
+        <v>44926</v>
+      </c>
+      <c r="L34" s="6">
+        <v>410000</v>
+      </c>
+      <c r="M34" s="6">
         <v>70000</v>
       </c>
       <c r="N34" s="20"/>
     </row>
-    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="29">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="B35" s="29" t="s">
         <v>175</v>
       </c>
       <c r="C35" s="4">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>173</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>191</v>
+        <v>56</v>
       </c>
       <c r="H35" s="8">
-        <v>264.23</v>
+        <v>1116.77</v>
       </c>
       <c r="I35" s="32" t="s">
         <v>3</v>
@@ -4720,22 +4712,14 @@
       <c r="J35" s="7">
         <v>44927</v>
       </c>
-      <c r="K35" s="5">
-        <v>49309</v>
-      </c>
-      <c r="L35" s="6">
-        <v>367500</v>
-      </c>
-      <c r="M35" s="6">
-        <v>70000</v>
-      </c>
-      <c r="N35" s="20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="K35" s="5"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="20"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="29">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B36" s="29" t="s">
         <v>175</v>
@@ -4744,82 +4728,70 @@
         <v>27</v>
       </c>
       <c r="D36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H36" s="8">
+        <v>289.7</v>
+      </c>
+      <c r="I36" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J36" s="7">
+        <v>45292</v>
+      </c>
+      <c r="K36" s="5"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="20"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="29">
         <v>36</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G36" s="3" t="s">
+      <c r="B37" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C37" s="4">
+        <v>27</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H37" s="8">
+        <v>137.66999999999999</v>
+      </c>
+      <c r="I37" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J37" s="7">
+        <v>45292</v>
+      </c>
+      <c r="K37" s="5"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="20"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="29">
         <v>37</v>
-      </c>
-      <c r="H36" s="8">
-        <v>1179.0999999999999</v>
-      </c>
-      <c r="I36" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="J36" s="7">
-        <v>43647</v>
-      </c>
-      <c r="K36" s="5">
-        <v>44926</v>
-      </c>
-      <c r="L36" s="6">
-        <v>410000</v>
-      </c>
-      <c r="M36" s="6">
-        <v>70000</v>
-      </c>
-      <c r="N36" s="20"/>
-    </row>
-    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="29">
-        <v>64</v>
-      </c>
-      <c r="B37" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="C37" s="4">
-        <v>17</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H37" s="8">
-        <v>1547.68451044725</v>
-      </c>
-      <c r="I37" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="J37" s="45">
-        <v>44986</v>
-      </c>
-      <c r="K37" s="5">
-        <v>49003</v>
-      </c>
-      <c r="L37" s="6">
-        <v>390000</v>
-      </c>
-      <c r="M37" s="6">
-        <v>70000</v>
-      </c>
-      <c r="N37" s="20"/>
-    </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="29">
-        <v>39</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>175</v>
@@ -4828,7 +4800,7 @@
         <v>26</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>173</v>
@@ -4837,31 +4809,31 @@
         <v>129</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H38" s="8">
-        <v>977.74</v>
+        <v>40</v>
+      </c>
+      <c r="H38" s="36">
+        <v>306.92</v>
       </c>
       <c r="I38" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J38" s="7">
-        <v>43678</v>
+      <c r="J38" s="39">
+        <v>44927</v>
       </c>
       <c r="K38" s="5">
-        <v>49156</v>
-      </c>
-      <c r="L38" s="6">
+        <v>49155</v>
+      </c>
+      <c r="L38" s="40">
         <v>367500</v>
       </c>
-      <c r="M38" s="6">
+      <c r="M38" s="40">
         <v>70000</v>
       </c>
       <c r="N38" s="20"/>
     </row>
-    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="29">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" s="29" t="s">
         <v>175</v>
@@ -4879,7 +4851,7 @@
         <v>182</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>13</v>
+        <v>179</v>
       </c>
       <c r="H39" s="8">
         <v>275.33</v>
@@ -4888,31 +4860,31 @@
         <v>3</v>
       </c>
       <c r="J39" s="7">
-        <v>44317</v>
+        <v>45413</v>
       </c>
       <c r="K39" s="5">
-        <v>45412</v>
+        <v>46507</v>
       </c>
       <c r="L39" s="6">
-        <v>440000</v>
+        <v>383000</v>
       </c>
       <c r="M39" s="6">
         <v>70000</v>
       </c>
       <c r="N39" s="20"/>
     </row>
-    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="29">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="B40" s="29" t="s">
         <v>175</v>
       </c>
       <c r="C40" s="4">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>173</v>
@@ -4921,33 +4893,31 @@
         <v>182</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>177</v>
+        <v>13</v>
       </c>
       <c r="H40" s="8">
-        <v>137.51</v>
+        <v>275.33</v>
       </c>
       <c r="I40" s="32" t="s">
         <v>3</v>
       </c>
       <c r="J40" s="7">
-        <v>45017</v>
+        <v>44317</v>
       </c>
       <c r="K40" s="5">
-        <v>49034</v>
+        <v>45412</v>
       </c>
       <c r="L40" s="6">
-        <v>410000</v>
+        <v>440000</v>
       </c>
       <c r="M40" s="6">
         <v>70000</v>
       </c>
-      <c r="N40" s="20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="N40" s="20"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="29">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B41" s="29" t="s">
         <v>175</v>
@@ -4987,18 +4957,18 @@
       </c>
       <c r="N41" s="20"/>
     </row>
-    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="29">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B42" s="29" t="s">
         <v>175</v>
       </c>
       <c r="C42" s="4">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>173</v>
@@ -5007,31 +4977,31 @@
         <v>129</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="H42" s="8">
-        <v>1623.88</v>
+        <v>977.74</v>
       </c>
       <c r="I42" s="32" t="s">
         <v>3</v>
       </c>
       <c r="J42" s="7">
-        <v>45108</v>
+        <v>43678</v>
       </c>
       <c r="K42" s="5">
-        <v>49125</v>
+        <v>49156</v>
       </c>
       <c r="L42" s="6">
-        <v>347396</v>
+        <v>367500</v>
       </c>
       <c r="M42" s="6">
-        <v>84100</v>
+        <v>70000</v>
       </c>
       <c r="N42" s="20"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="29">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B43" s="29" t="s">
         <v>175</v>
@@ -5040,7 +5010,7 @@
         <v>25</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>173</v>
@@ -5049,286 +5019,282 @@
         <v>129</v>
       </c>
       <c r="G43" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H43" s="8">
+        <v>137.71</v>
+      </c>
+      <c r="I43" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J43" s="7">
+        <v>44682</v>
+      </c>
+      <c r="K43" s="5">
+        <v>49064</v>
+      </c>
+      <c r="L43" s="6">
+        <v>383000</v>
+      </c>
+      <c r="M43" s="6">
+        <v>70000</v>
+      </c>
+      <c r="N43" s="20"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" s="29">
+        <v>43</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C44" s="4">
+        <v>25</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H44" s="8">
+        <v>306.92</v>
+      </c>
+      <c r="I44" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J44" s="7">
+        <v>43191</v>
+      </c>
+      <c r="K44" s="5">
+        <v>45382</v>
+      </c>
+      <c r="L44" s="6">
+        <v>383000</v>
+      </c>
+      <c r="M44" s="6">
+        <v>70000</v>
+      </c>
+      <c r="N44" s="20"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" s="29">
+        <v>44</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C45" s="4">
+        <v>25</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G45" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H45" s="43">
+        <v>137.66999999999999</v>
+      </c>
+      <c r="I45" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J45" s="7">
+        <v>43282</v>
+      </c>
+      <c r="K45" s="5">
+        <v>44926</v>
+      </c>
+      <c r="L45" s="6">
+        <v>410000</v>
+      </c>
+      <c r="M45" s="40">
+        <v>70000</v>
+      </c>
+      <c r="N45" s="20"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" s="29">
+        <v>45</v>
+      </c>
+      <c r="B46" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C46" s="4">
+        <v>25</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="H46" s="43">
+        <v>137.66999999999999</v>
+      </c>
+      <c r="I46" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J46" s="7">
+        <v>45658</v>
+      </c>
+      <c r="K46" s="5">
+        <v>49309</v>
+      </c>
+      <c r="L46" s="6">
+        <v>400000</v>
+      </c>
+      <c r="M46" s="40">
+        <v>70000</v>
+      </c>
+      <c r="N46" s="20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" s="29">
+        <v>46</v>
+      </c>
+      <c r="B47" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C47" s="4">
+        <v>25</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H47" s="8">
+        <v>137.66999999999999</v>
+      </c>
+      <c r="I47" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J47" s="7">
+        <v>45383</v>
+      </c>
+      <c r="K47" s="5"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="20"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" s="29">
+        <v>47</v>
+      </c>
+      <c r="B48" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C48" s="4">
+        <v>25</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H48" s="8">
+        <v>306.92</v>
+      </c>
+      <c r="I48" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J48" s="7">
+        <v>45383</v>
+      </c>
+      <c r="K48" s="5">
+        <v>49034</v>
+      </c>
+      <c r="L48" s="6">
+        <v>383000</v>
+      </c>
+      <c r="M48" s="6">
+        <v>70000</v>
+      </c>
+      <c r="N48" s="20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" s="29">
+        <v>48</v>
+      </c>
+      <c r="B49" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C49" s="4">
+        <v>25</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G49" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H43" s="8">
+      <c r="H49" s="8">
         <v>439.08</v>
       </c>
-      <c r="I43" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="J43" s="7">
+      <c r="I49" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J49" s="7">
         <v>43739</v>
       </c>
-      <c r="K43" s="5">
+      <c r="K49" s="5">
         <v>45291</v>
       </c>
-      <c r="L43" s="6">
+      <c r="L49" s="6">
         <f>362500*11.5/12</f>
         <v>347395.83333333331</v>
       </c>
-      <c r="M43" s="6">
+      <c r="M49" s="6">
         <v>84100</v>
-      </c>
-      <c r="N43" s="20"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="29">
-        <v>42</v>
-      </c>
-      <c r="B44" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="C44" s="4">
-        <v>25</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G44" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="H44" s="43">
-        <v>137.66999999999999</v>
-      </c>
-      <c r="I44" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="J44" s="7">
-        <v>43282</v>
-      </c>
-      <c r="K44" s="5">
-        <v>44926</v>
-      </c>
-      <c r="L44" s="6">
-        <v>410000</v>
-      </c>
-      <c r="M44" s="40">
-        <v>70000</v>
-      </c>
-      <c r="N44" s="20"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="29">
-        <v>43</v>
-      </c>
-      <c r="B45" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="C45" s="4">
-        <v>25</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G45" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="H45" s="43">
-        <v>137.66999999999999</v>
-      </c>
-      <c r="I45" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="J45" s="7">
-        <v>45658</v>
-      </c>
-      <c r="K45" s="5">
-        <v>49309</v>
-      </c>
-      <c r="L45" s="6">
-        <v>400000</v>
-      </c>
-      <c r="M45" s="40">
-        <v>70000</v>
-      </c>
-      <c r="N45" s="20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="29">
-        <v>48</v>
-      </c>
-      <c r="B46" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="C46" s="4">
-        <v>23</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H46" s="8">
-        <v>1547.71</v>
-      </c>
-      <c r="I46" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="J46" s="7">
-        <v>45108</v>
-      </c>
-      <c r="K46" s="5">
-        <v>49125</v>
-      </c>
-      <c r="L46" s="6">
-        <v>347396</v>
-      </c>
-      <c r="M46" s="6">
-        <v>84100</v>
-      </c>
-      <c r="N46" s="20"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A47" s="29">
-        <v>41</v>
-      </c>
-      <c r="B47" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="C47" s="4">
-        <v>25</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H47" s="8">
-        <v>306.92</v>
-      </c>
-      <c r="I47" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="J47" s="7">
-        <v>43191</v>
-      </c>
-      <c r="K47" s="5">
-        <v>45382</v>
-      </c>
-      <c r="L47" s="6">
-        <v>383000</v>
-      </c>
-      <c r="M47" s="6">
-        <v>70000</v>
-      </c>
-      <c r="N47" s="20"/>
-    </row>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="29">
-        <v>50</v>
-      </c>
-      <c r="B48" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="C48" s="4">
-        <v>21</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H48" s="8">
-        <v>1547.7674437292999</v>
-      </c>
-      <c r="I48" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="J48" s="7">
-        <v>45108</v>
-      </c>
-      <c r="K48" s="5">
-        <v>49125</v>
-      </c>
-      <c r="L48" s="6">
-        <v>347396</v>
-      </c>
-      <c r="M48" s="6">
-        <v>84100</v>
-      </c>
-      <c r="N48" s="20"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A49" s="29">
-        <v>47</v>
-      </c>
-      <c r="B49" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="C49" s="4">
-        <v>25</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H49" s="8">
-        <v>388.65999999999997</v>
-      </c>
-      <c r="I49" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="J49" s="7">
-        <v>43739</v>
-      </c>
-      <c r="K49" s="5">
-        <v>49217</v>
-      </c>
-      <c r="L49" s="6">
-        <v>383000</v>
-      </c>
-      <c r="M49" s="6">
-        <v>70000</v>
       </c>
       <c r="N49" s="20"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="29">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B50" s="29" t="s">
         <v>175</v>
@@ -5337,7 +5303,7 @@
         <v>25</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>173</v>
@@ -5349,16 +5315,16 @@
         <v>43</v>
       </c>
       <c r="H50" s="8">
-        <v>137.71</v>
+        <v>388.65999999999997</v>
       </c>
       <c r="I50" s="32" t="s">
         <v>3</v>
       </c>
       <c r="J50" s="7">
-        <v>44682</v>
+        <v>43739</v>
       </c>
       <c r="K50" s="5">
-        <v>49064</v>
+        <v>49217</v>
       </c>
       <c r="L50" s="6">
         <v>383000</v>
@@ -5368,28 +5334,30 @@
       </c>
       <c r="N50" s="20"/>
     </row>
-    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="29"/>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" s="29">
+        <v>50</v>
+      </c>
       <c r="B51" s="29" t="s">
         <v>175</v>
       </c>
       <c r="C51" s="4">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>173</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>182</v>
+        <v>129</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>177</v>
+        <v>47</v>
       </c>
       <c r="H51" s="8">
-        <v>272.08</v>
+        <v>1547.71</v>
       </c>
       <c r="I51" s="32" t="s">
         <v>3</v>
@@ -5397,22 +5365,20 @@
       <c r="J51" s="7">
         <v>45108</v>
       </c>
-      <c r="K51" s="45">
+      <c r="K51" s="5">
         <v>49125</v>
       </c>
       <c r="L51" s="6">
-        <v>383000</v>
+        <v>347396</v>
       </c>
       <c r="M51" s="6">
-        <v>70000</v>
-      </c>
-      <c r="N51" s="20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>84100</v>
+      </c>
+      <c r="N51" s="20"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="29">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B52" s="29" t="s">
         <v>175</v>
@@ -5452,30 +5418,30 @@
       </c>
       <c r="N52" s="20"/>
     </row>
-    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="29">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="B53" s="29" t="s">
         <v>175</v>
       </c>
       <c r="C53" s="4">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>173</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>182</v>
+        <v>129</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H53" s="8">
-        <v>272.08</v>
+        <v>1547.7674437292999</v>
       </c>
       <c r="I53" s="32" t="s">
         <v>3</v>
@@ -5483,14 +5449,20 @@
       <c r="J53" s="7">
         <v>45108</v>
       </c>
-      <c r="K53" s="45"/>
-      <c r="L53" s="6"/>
-      <c r="M53" s="6"/>
+      <c r="K53" s="5">
+        <v>49125</v>
+      </c>
+      <c r="L53" s="6">
+        <v>347396</v>
+      </c>
+      <c r="M53" s="6">
+        <v>84100</v>
+      </c>
       <c r="N53" s="20"/>
     </row>
-    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="29">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B54" s="29" t="s">
         <v>175</v>
@@ -5531,9 +5503,9 @@
       </c>
       <c r="N54" s="20"/>
     </row>
-    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="29">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B55" s="29" t="s">
         <v>175</v>
@@ -5551,31 +5523,31 @@
         <v>182</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H55" s="8">
+        <v>49</v>
+      </c>
+      <c r="H55" s="34">
         <v>651.25</v>
       </c>
       <c r="I55" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J55" s="7">
-        <v>43206</v>
+      <c r="J55" s="5">
+        <v>45763</v>
       </c>
       <c r="K55" s="5">
-        <v>45762</v>
+        <v>49049</v>
       </c>
       <c r="L55" s="6">
-        <v>420000</v>
+        <v>383000</v>
       </c>
       <c r="M55" s="6">
         <v>70000</v>
       </c>
       <c r="N55" s="20"/>
     </row>
-    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="29">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B56" s="29" t="s">
         <v>175</v>
@@ -5593,31 +5565,31 @@
         <v>182</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H56" s="34">
+        <v>48</v>
+      </c>
+      <c r="H56" s="8">
         <v>651.25</v>
       </c>
       <c r="I56" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J56" s="5">
-        <v>45763</v>
+      <c r="J56" s="7">
+        <v>43206</v>
       </c>
       <c r="K56" s="5">
-        <v>49049</v>
+        <v>45762</v>
       </c>
       <c r="L56" s="6">
-        <v>383000</v>
+        <v>420000</v>
       </c>
       <c r="M56" s="6">
         <v>70000</v>
       </c>
       <c r="N56" s="20"/>
     </row>
-    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="29">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B57" s="29" t="s">
         <v>175</v>
@@ -5626,7 +5598,7 @@
         <v>20</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>173</v>
@@ -5635,25 +5607,31 @@
         <v>182</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H57" s="34">
-        <v>250.99</v>
+        <v>51</v>
+      </c>
+      <c r="H57" s="8">
+        <v>137.67083232602312</v>
       </c>
       <c r="I57" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J57" s="5">
-        <v>44562</v>
-      </c>
-      <c r="K57" s="5"/>
-      <c r="L57" s="6"/>
-      <c r="M57" s="6"/>
+      <c r="J57" s="44">
+        <v>44197</v>
+      </c>
+      <c r="K57" s="5">
+        <v>45291</v>
+      </c>
+      <c r="L57" s="6">
+        <v>430000</v>
+      </c>
+      <c r="M57" s="6">
+        <v>70000</v>
+      </c>
       <c r="N57" s="20"/>
     </row>
-    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="29">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B58" s="29" t="s">
         <v>175</v>
@@ -5662,82 +5640,76 @@
         <v>20</v>
       </c>
       <c r="D58" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H58" s="34">
+        <v>250.99</v>
+      </c>
+      <c r="I58" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J58" s="5">
+        <v>44562</v>
+      </c>
+      <c r="K58" s="5"/>
+      <c r="L58" s="6"/>
+      <c r="M58" s="6"/>
+      <c r="N58" s="20"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59" s="29">
+        <v>58</v>
+      </c>
+      <c r="B59" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C59" s="4">
+        <v>20</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E58" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H58" s="8">
+      <c r="E59" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="H59" s="8">
         <v>137.67083232602312</v>
       </c>
-      <c r="I58" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="J58" s="44">
-        <v>44197</v>
-      </c>
-      <c r="K58" s="5">
-        <v>45291</v>
-      </c>
-      <c r="L58" s="6">
-        <v>430000</v>
-      </c>
-      <c r="M58" s="6">
-        <v>70000</v>
-      </c>
-      <c r="N58" s="20"/>
-    </row>
-    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="29">
-        <v>69</v>
-      </c>
-      <c r="B59" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="C59" s="4">
-        <v>15</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H59" s="8">
-        <v>1547.75</v>
-      </c>
       <c r="I59" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="J59" s="7">
-        <v>45139</v>
+      <c r="J59" s="44">
+        <v>45292</v>
       </c>
       <c r="K59" s="5">
-        <v>49156</v>
+        <v>46752</v>
       </c>
       <c r="L59" s="6">
-        <v>390000</v>
+        <v>410000</v>
       </c>
       <c r="M59" s="6">
         <v>70000</v>
       </c>
       <c r="N59" s="20"/>
     </row>
-    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="29">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B60" s="29" t="s">
         <v>175</v>
@@ -5771,9 +5743,9 @@
       <c r="M60" s="6"/>
       <c r="N60" s="20"/>
     </row>
-    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="29">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B61" s="29" t="s">
         <v>175</v>
@@ -5813,9 +5785,9 @@
       </c>
       <c r="N61" s="20"/>
     </row>
-    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="29">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B62" s="29" t="s">
         <v>175</v>
@@ -5824,7 +5796,7 @@
         <v>19</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>173</v>
@@ -5833,31 +5805,31 @@
         <v>182</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H62" s="8">
-        <v>989.79</v>
+        <v>306.92</v>
       </c>
       <c r="I62" s="32" t="s">
         <v>3</v>
       </c>
       <c r="J62" s="7">
-        <v>45170</v>
+        <v>43449</v>
       </c>
       <c r="K62" s="5">
-        <v>49187</v>
+        <v>44544</v>
       </c>
       <c r="L62" s="6">
-        <v>400000</v>
+        <v>383000</v>
       </c>
       <c r="M62" s="6">
         <v>70000</v>
       </c>
       <c r="N62" s="20"/>
     </row>
-    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="29">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B63" s="29" t="s">
         <v>175</v>
@@ -5866,7 +5838,7 @@
         <v>19</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>173</v>
@@ -5875,30 +5847,32 @@
         <v>182</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H63" s="8">
-        <v>306.92</v>
+        <v>989.79</v>
       </c>
       <c r="I63" s="32" t="s">
         <v>3</v>
       </c>
       <c r="J63" s="7">
-        <v>43449</v>
+        <v>45170</v>
       </c>
       <c r="K63" s="5">
-        <v>44544</v>
+        <v>49187</v>
       </c>
       <c r="L63" s="6">
-        <v>383000</v>
+        <v>400000</v>
       </c>
       <c r="M63" s="6">
         <v>70000</v>
       </c>
       <c r="N63" s="20"/>
     </row>
-    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="29"/>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" s="29">
+        <v>63</v>
+      </c>
       <c r="B64" s="29" t="s">
         <v>175</v>
       </c>
@@ -5906,7 +5880,7 @@
         <v>19</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>173</v>
@@ -5915,25 +5889,31 @@
         <v>182</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H64" s="8">
-        <v>306.92</v>
+        <v>250.99</v>
       </c>
       <c r="I64" s="32" t="s">
         <v>3</v>
       </c>
       <c r="J64" s="7">
-        <v>44545</v>
-      </c>
-      <c r="K64" s="5"/>
-      <c r="L64" s="6"/>
-      <c r="M64" s="6"/>
+        <v>45170</v>
+      </c>
+      <c r="K64" s="5">
+        <v>49187</v>
+      </c>
+      <c r="L64" s="6">
+        <v>400000</v>
+      </c>
+      <c r="M64" s="6">
+        <v>70000</v>
+      </c>
       <c r="N64" s="20"/>
     </row>
-    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="29">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B65" s="29" t="s">
         <v>175</v>
@@ -5942,7 +5922,7 @@
         <v>19</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>173</v>
@@ -5951,31 +5931,25 @@
         <v>182</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H65" s="8">
-        <v>250.99</v>
+        <v>306.92</v>
       </c>
       <c r="I65" s="32" t="s">
         <v>3</v>
       </c>
       <c r="J65" s="7">
-        <v>45170</v>
-      </c>
-      <c r="K65" s="5">
-        <v>49187</v>
-      </c>
-      <c r="L65" s="6">
-        <v>400000</v>
-      </c>
-      <c r="M65" s="6">
-        <v>70000</v>
-      </c>
+        <v>44545</v>
+      </c>
+      <c r="K65" s="5"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
       <c r="N65" s="20"/>
     </row>
-    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="29">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B66" s="29" t="s">
         <v>175</v>
@@ -6015,9 +5989,9 @@
       </c>
       <c r="N66" s="20"/>
     </row>
-    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="29">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B67" s="29" t="s">
         <v>175</v>
@@ -6035,29 +6009,29 @@
         <v>182</v>
       </c>
       <c r="G67" s="59" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H67" s="62">
-        <v>1547.6845104472457</v>
+        <v>1547.68451044725</v>
       </c>
       <c r="I67" s="67" t="s">
         <v>3</v>
       </c>
       <c r="J67" s="54">
-        <v>43891</v>
+        <v>44986</v>
       </c>
       <c r="K67" s="71">
-        <v>44985</v>
+        <v>49003</v>
       </c>
       <c r="L67" s="73">
-        <v>450000</v>
+        <v>390000</v>
       </c>
       <c r="M67" s="6">
         <v>70000</v>
       </c>
       <c r="N67" s="20"/>
     </row>
-    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="29">
         <v>67</v>
       </c>
@@ -6065,7 +6039,7 @@
         <v>175</v>
       </c>
       <c r="C68" s="58">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D68" s="58" t="s">
         <v>18</v>
@@ -6077,31 +6051,31 @@
         <v>182</v>
       </c>
       <c r="G68" s="59" t="s">
-        <v>189</v>
+        <v>57</v>
       </c>
       <c r="H68" s="62">
-        <v>1559.07</v>
+        <v>1547.6845104472457</v>
       </c>
       <c r="I68" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="J68" s="69">
-        <v>45170</v>
+      <c r="J68" s="54">
+        <v>43891</v>
       </c>
       <c r="K68" s="71">
-        <v>49187</v>
+        <v>44985</v>
       </c>
       <c r="L68" s="73">
-        <v>400000</v>
+        <v>450000</v>
       </c>
       <c r="M68" s="6">
         <v>70000</v>
       </c>
       <c r="N68" s="20"/>
     </row>
-    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="29">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B69" s="29" t="s">
         <v>175</v>
@@ -6141,18 +6115,18 @@
       </c>
       <c r="N69" s="20"/>
     </row>
-    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="29">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B70" s="29" t="s">
         <v>175</v>
       </c>
       <c r="C70" s="58">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D70" s="58" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E70" s="57" t="s">
         <v>173</v>
@@ -6161,33 +6135,31 @@
         <v>182</v>
       </c>
       <c r="G70" s="59" t="s">
-        <v>123</v>
+        <v>189</v>
       </c>
       <c r="H70" s="62">
-        <v>135.97999999999999</v>
+        <v>1559.07</v>
       </c>
       <c r="I70" s="67" t="s">
         <v>3</v>
       </c>
       <c r="J70" s="69">
-        <v>45184</v>
+        <v>45170</v>
       </c>
       <c r="K70" s="71">
-        <v>49201</v>
+        <v>49187</v>
       </c>
       <c r="L70" s="73">
-        <v>390000</v>
+        <v>400000</v>
       </c>
       <c r="M70" s="6">
         <v>70000</v>
       </c>
-      <c r="N70" s="20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="N70" s="20"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="29">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B71" s="29" t="s">
         <v>175</v>
@@ -6227,51 +6199,51 @@
       </c>
       <c r="N71" s="20"/>
     </row>
-    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="29">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="B72" s="29" t="s">
         <v>175</v>
       </c>
       <c r="C72" s="58">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D72" s="58" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="E72" s="57" t="s">
         <v>173</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="G72" s="59" t="s">
-        <v>176</v>
+        <v>60</v>
       </c>
       <c r="H72" s="62">
-        <v>1234.75</v>
+        <v>1547.75</v>
       </c>
       <c r="I72" s="67" t="s">
         <v>3</v>
       </c>
       <c r="J72" s="69">
-        <v>45200</v>
+        <v>45139</v>
       </c>
       <c r="K72" s="71">
-        <v>49308</v>
+        <v>49156</v>
       </c>
       <c r="L72" s="73">
-        <v>367500</v>
+        <v>390000</v>
       </c>
       <c r="M72" s="6">
         <v>70000</v>
       </c>
       <c r="N72" s="20"/>
     </row>
-    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="29">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B73" s="29" t="s">
         <v>175</v>
@@ -6311,9 +6283,9 @@
       </c>
       <c r="N73" s="20"/>
     </row>
-    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="29">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B74" s="29" t="s">
         <v>175</v>
@@ -6347,9 +6319,9 @@
       <c r="M74" s="6"/>
       <c r="N74" s="20"/>
     </row>
-    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="29">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B75" s="29" t="s">
         <v>175</v>
@@ -6389,9 +6361,9 @@
       </c>
       <c r="N75" s="20"/>
     </row>
-    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="29">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B76" s="29" t="s">
         <v>175</v>
@@ -6433,9 +6405,9 @@
         <v>186</v>
       </c>
     </row>
-    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="29">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" s="29" t="s">
         <v>175</v>
@@ -6453,7 +6425,7 @@
         <v>182</v>
       </c>
       <c r="G77" s="59" t="s">
-        <v>184</v>
+        <v>116</v>
       </c>
       <c r="H77" s="62">
         <v>287.33999999999997</v>
@@ -6462,29 +6434,31 @@
         <v>3</v>
       </c>
       <c r="J77" s="69">
-        <v>44136</v>
+        <v>45352</v>
       </c>
       <c r="K77" s="71">
-        <v>45350</v>
+        <v>49003</v>
       </c>
       <c r="L77" s="73">
-        <v>425000</v>
+        <v>400000</v>
       </c>
       <c r="M77" s="6">
         <v>70000</v>
       </c>
       <c r="N77" s="20"/>
     </row>
-    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="29"/>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A78" s="29">
+        <v>77</v>
+      </c>
       <c r="B78" s="29" t="s">
         <v>175</v>
       </c>
       <c r="C78" s="58">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D78" s="58" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E78" s="57" t="s">
         <v>173</v>
@@ -6493,25 +6467,33 @@
         <v>182</v>
       </c>
       <c r="G78" s="59" t="s">
-        <v>56</v>
+        <v>123</v>
       </c>
       <c r="H78" s="62">
-        <v>289.7</v>
+        <v>135.97999999999999</v>
       </c>
       <c r="I78" s="67" t="s">
         <v>3</v>
       </c>
       <c r="J78" s="69">
-        <v>45292</v>
-      </c>
-      <c r="K78" s="71"/>
-      <c r="L78" s="73"/>
-      <c r="M78" s="6"/>
-      <c r="N78" s="20"/>
-    </row>
-    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>45184</v>
+      </c>
+      <c r="K78" s="71">
+        <v>49201</v>
+      </c>
+      <c r="L78" s="73">
+        <v>390000</v>
+      </c>
+      <c r="M78" s="6">
+        <v>70000</v>
+      </c>
+      <c r="N78" s="20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="29">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B79" s="29" t="s">
         <v>175</v>
@@ -6520,7 +6502,7 @@
         <v>10</v>
       </c>
       <c r="D79" s="58" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="E79" s="57" t="s">
         <v>173</v>
@@ -6532,20 +6514,20 @@
         <v>56</v>
       </c>
       <c r="H79" s="62">
-        <v>287.33999999999997</v>
+        <v>272.08</v>
       </c>
       <c r="I79" s="67" t="s">
         <v>3</v>
       </c>
       <c r="J79" s="69">
-        <v>46813</v>
-      </c>
-      <c r="K79" s="71"/>
+        <v>45108</v>
+      </c>
+      <c r="K79" s="54"/>
       <c r="L79" s="73"/>
       <c r="M79" s="6"/>
       <c r="N79" s="20"/>
     </row>
-    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="29">
         <v>79</v>
       </c>
@@ -6556,7 +6538,7 @@
         <v>10</v>
       </c>
       <c r="D80" s="58" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E80" s="57" t="s">
         <v>173</v>
@@ -6565,65 +6547,73 @@
         <v>182</v>
       </c>
       <c r="G80" s="59" t="s">
-        <v>63</v>
+        <v>184</v>
       </c>
       <c r="H80" s="62">
-        <v>135.97999999999999</v>
+        <v>287.33999999999997</v>
       </c>
       <c r="I80" s="67" t="s">
         <v>3</v>
       </c>
       <c r="J80" s="69">
-        <v>44089</v>
+        <v>44136</v>
       </c>
       <c r="K80" s="71">
-        <v>45183</v>
+        <v>45350</v>
       </c>
       <c r="L80" s="73">
-        <v>435000</v>
+        <v>425000</v>
       </c>
       <c r="M80" s="6">
         <v>70000</v>
       </c>
       <c r="N80" s="20"/>
     </row>
-    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="29"/>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A81" s="29">
+        <v>80</v>
+      </c>
       <c r="B81" s="29" t="s">
         <v>175</v>
       </c>
       <c r="C81" s="58">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D81" s="58" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E81" s="57" t="s">
         <v>173</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>182</v>
+        <v>129</v>
       </c>
       <c r="G81" s="59" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="H81" s="62">
-        <v>137.66999999999999</v>
+        <v>264.23</v>
       </c>
       <c r="I81" s="67" t="s">
         <v>3</v>
       </c>
       <c r="J81" s="69">
-        <v>45292</v>
-      </c>
-      <c r="K81" s="71"/>
-      <c r="L81" s="73"/>
-      <c r="M81" s="6"/>
+        <v>44835</v>
+      </c>
+      <c r="K81" s="71">
+        <v>44926</v>
+      </c>
+      <c r="L81" s="73">
+        <v>367500</v>
+      </c>
+      <c r="M81" s="6">
+        <v>70000</v>
+      </c>
       <c r="N81" s="20"/>
     </row>
-    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="29">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B82" s="29" t="s">
         <v>175</v>
@@ -6641,7 +6631,7 @@
         <v>182</v>
       </c>
       <c r="G82" s="59" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="H82" s="62">
         <v>135.97999999999999</v>
@@ -6650,16 +6640,22 @@
         <v>3</v>
       </c>
       <c r="J82" s="69">
-        <v>46280</v>
-      </c>
-      <c r="K82" s="71"/>
-      <c r="L82" s="73"/>
-      <c r="M82" s="6"/>
+        <v>44089</v>
+      </c>
+      <c r="K82" s="71">
+        <v>45183</v>
+      </c>
+      <c r="L82" s="73">
+        <v>435000</v>
+      </c>
+      <c r="M82" s="6">
+        <v>70000</v>
+      </c>
       <c r="N82" s="20"/>
     </row>
-    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="29">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B83" s="29" t="s">
         <v>175</v>
@@ -6668,38 +6664,41 @@
         <v>10</v>
       </c>
       <c r="D83" s="58" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E83" s="57" t="s">
         <v>173</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>182</v>
+        <v>129</v>
       </c>
       <c r="G83" s="59" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="H83" s="62">
-        <v>135.99</v>
+        <v>264.23</v>
       </c>
       <c r="I83" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="J83" s="69"/>
+      <c r="J83" s="69">
+        <v>43647</v>
+      </c>
       <c r="K83" s="71">
-        <v>49187</v>
+        <v>44561</v>
       </c>
       <c r="L83" s="73">
-        <v>0</v>
+        <f>362500*11.5/12</f>
+        <v>347395.83333333331</v>
       </c>
       <c r="M83" s="6">
-        <v>0</v>
+        <v>84100</v>
       </c>
       <c r="N83" s="20"/>
     </row>
-    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="29">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B84" s="29" t="s">
         <v>175</v>
@@ -6708,7 +6707,7 @@
         <v>10</v>
       </c>
       <c r="D84" s="58" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E84" s="57" t="s">
         <v>173</v>
@@ -6717,71 +6716,61 @@
         <v>182</v>
       </c>
       <c r="G84" s="59" t="s">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="H84" s="62">
-        <v>392.7</v>
+        <v>287.33999999999997</v>
       </c>
       <c r="I84" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="J84" s="69"/>
-      <c r="K84" s="71">
-        <v>49187</v>
-      </c>
-      <c r="L84" s="73">
-        <v>0</v>
-      </c>
-      <c r="M84" s="6">
-        <v>0</v>
-      </c>
+      <c r="J84" s="69">
+        <v>46813</v>
+      </c>
+      <c r="K84" s="71"/>
+      <c r="L84" s="73"/>
+      <c r="M84" s="6"/>
       <c r="N84" s="20"/>
     </row>
-    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="29">
+        <v>84</v>
+      </c>
+      <c r="B85" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C85" s="58">
+        <v>10</v>
+      </c>
+      <c r="D85" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="E85" s="57" t="s">
+        <v>173</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G85" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="B85" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="C85" s="58">
-        <v>20</v>
-      </c>
-      <c r="D85" s="58" t="s">
-        <v>8</v>
-      </c>
-      <c r="E85" s="57" t="s">
-        <v>173</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G85" s="59" t="s">
-        <v>190</v>
-      </c>
       <c r="H85" s="62">
-        <v>137.67083232602312</v>
+        <v>135.97999999999999</v>
       </c>
       <c r="I85" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="J85" s="85">
-        <v>45292</v>
-      </c>
-      <c r="K85" s="71">
-        <v>46752</v>
-      </c>
-      <c r="L85" s="73">
-        <v>410000</v>
-      </c>
-      <c r="M85" s="6">
-        <v>70000</v>
-      </c>
+      <c r="J85" s="69">
+        <v>46280</v>
+      </c>
+      <c r="K85" s="71"/>
+      <c r="L85" s="73"/>
+      <c r="M85" s="6"/>
       <c r="N85" s="20"/>
     </row>
-    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="29">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B86" s="29" t="s">
         <v>175</v>
@@ -6790,40 +6779,42 @@
         <v>10</v>
       </c>
       <c r="D86" s="58" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E86" s="57" t="s">
         <v>173</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>182</v>
+        <v>129</v>
       </c>
       <c r="G86" s="59" t="s">
-        <v>116</v>
+        <v>191</v>
       </c>
       <c r="H86" s="62">
-        <v>287.33999999999997</v>
+        <v>264.23</v>
       </c>
       <c r="I86" s="67" t="s">
         <v>3</v>
       </c>
       <c r="J86" s="69">
-        <v>45352</v>
+        <v>44927</v>
       </c>
       <c r="K86" s="71">
-        <v>49003</v>
+        <v>49309</v>
       </c>
       <c r="L86" s="73">
-        <v>400000</v>
+        <v>367500</v>
       </c>
       <c r="M86" s="6">
         <v>70000</v>
       </c>
-      <c r="N86" s="20"/>
-    </row>
-    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="N86" s="20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="29">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B87" s="29" t="s">
         <v>175</v>
@@ -6832,41 +6823,38 @@
         <v>10</v>
       </c>
       <c r="D87" s="58" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E87" s="57" t="s">
         <v>173</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="G87" s="59" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="H87" s="62">
-        <v>264.23</v>
+        <v>135.99</v>
       </c>
       <c r="I87" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="J87" s="69">
-        <v>43647</v>
-      </c>
+      <c r="J87" s="69"/>
       <c r="K87" s="71">
-        <v>44561</v>
+        <v>49187</v>
       </c>
       <c r="L87" s="73">
-        <f>362500*11.5/12</f>
-        <v>347395.83333333331</v>
+        <v>0</v>
       </c>
       <c r="M87" s="6">
-        <v>84100</v>
+        <v>0</v>
       </c>
       <c r="N87" s="20"/>
     </row>
-    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="29">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B88" s="29" t="s">
         <v>175</v>
@@ -6875,49 +6863,47 @@
         <v>10</v>
       </c>
       <c r="D88" s="58" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E88" s="57" t="s">
         <v>173</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="G88" s="59" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="H88" s="62">
-        <v>264.23</v>
+        <v>392.7</v>
       </c>
       <c r="I88" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="J88" s="69">
-        <v>44835</v>
-      </c>
+      <c r="J88" s="69"/>
       <c r="K88" s="71">
-        <v>44926</v>
+        <v>49187</v>
       </c>
       <c r="L88" s="73">
-        <v>367500</v>
+        <v>0</v>
       </c>
       <c r="M88" s="6">
-        <v>70000</v>
+        <v>0</v>
       </c>
       <c r="N88" s="20"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="29">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="B89" s="29" t="s">
         <v>175</v>
       </c>
       <c r="C89" s="58">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D89" s="58" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="E89" s="57" t="s">
         <v>173</v>
@@ -6926,25 +6912,33 @@
         <v>182</v>
       </c>
       <c r="G89" s="59" t="s">
-        <v>56</v>
+        <v>177</v>
       </c>
       <c r="H89" s="62">
-        <v>137.66999999999999</v>
+        <v>272.08</v>
       </c>
       <c r="I89" s="67" t="s">
         <v>3</v>
       </c>
       <c r="J89" s="69">
-        <v>45383</v>
-      </c>
-      <c r="K89" s="71"/>
-      <c r="L89" s="73"/>
-      <c r="M89" s="6"/>
-      <c r="N89" s="20"/>
-    </row>
-    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>45108</v>
+      </c>
+      <c r="K89" s="54">
+        <v>49125</v>
+      </c>
+      <c r="L89" s="73">
+        <v>383000</v>
+      </c>
+      <c r="M89" s="6">
+        <v>70000</v>
+      </c>
+      <c r="N89" s="20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="29">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B90" s="29" t="s">
         <v>175</v>
@@ -6953,7 +6947,7 @@
         <v>9</v>
       </c>
       <c r="D90" s="58" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="E90" s="57" t="s">
         <v>173</v>
@@ -6962,28 +6956,34 @@
         <v>182</v>
       </c>
       <c r="G90" s="59" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H90" s="62">
-        <v>1234.75</v>
+        <v>137.52000000000001</v>
       </c>
       <c r="I90" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="J90" s="69"/>
+      <c r="J90" s="69">
+        <v>45566</v>
+      </c>
       <c r="K90" s="71">
-        <v>44895</v>
+        <v>49217</v>
       </c>
       <c r="L90" s="73">
-        <v>390000</v>
+        <v>0</v>
       </c>
       <c r="M90" s="6">
         <v>70000</v>
       </c>
-      <c r="N90" s="20"/>
-    </row>
-    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="29"/>
+      <c r="N90" s="20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A91" s="29">
+        <v>90</v>
+      </c>
       <c r="B91" s="29" t="s">
         <v>175</v>
       </c>
@@ -6991,7 +6991,7 @@
         <v>9</v>
       </c>
       <c r="D91" s="58" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="E91" s="57" t="s">
         <v>173</v>
@@ -7000,34 +7000,40 @@
         <v>182</v>
       </c>
       <c r="G91" s="59" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="H91" s="62">
-        <v>1234.75</v>
+        <v>137.52000000000001</v>
       </c>
       <c r="I91" s="67" t="s">
         <v>3</v>
       </c>
       <c r="J91" s="69">
-        <v>44896</v>
-      </c>
-      <c r="K91" s="71"/>
-      <c r="L91" s="73"/>
-      <c r="M91" s="6"/>
+        <v>43717</v>
+      </c>
+      <c r="K91" s="71">
+        <v>45565</v>
+      </c>
+      <c r="L91" s="73">
+        <v>0</v>
+      </c>
+      <c r="M91" s="6">
+        <v>70000</v>
+      </c>
       <c r="N91" s="20"/>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="29">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="B92" s="29" t="s">
         <v>175</v>
       </c>
       <c r="C92" s="58">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D92" s="58" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E92" s="57" t="s">
         <v>173</v>
@@ -7036,22 +7042,22 @@
         <v>182</v>
       </c>
       <c r="G92" s="59" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="H92" s="62">
-        <v>306.92</v>
+        <v>137.51</v>
       </c>
       <c r="I92" s="67" t="s">
         <v>3</v>
       </c>
       <c r="J92" s="69">
-        <v>45383</v>
+        <v>45017</v>
       </c>
       <c r="K92" s="71">
         <v>49034</v>
       </c>
       <c r="L92" s="73">
-        <v>383000</v>
+        <v>410000</v>
       </c>
       <c r="M92" s="6">
         <v>70000</v>
@@ -7060,9 +7066,9 @@
         <v>186</v>
       </c>
     </row>
-    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="29">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B93" s="29" t="s">
         <v>175</v>
@@ -7102,18 +7108,18 @@
       </c>
       <c r="N93" s="20"/>
     </row>
-    <row r="94" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="29">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="B94" s="29" t="s">
         <v>175</v>
       </c>
       <c r="C94" s="58">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D94" s="58" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="E94" s="57" t="s">
         <v>173</v>
@@ -7122,31 +7128,29 @@
         <v>182</v>
       </c>
       <c r="G94" s="59" t="s">
-        <v>179</v>
+        <v>68</v>
       </c>
       <c r="H94" s="62">
-        <v>275.33</v>
+        <v>1234.75</v>
       </c>
       <c r="I94" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="J94" s="69">
-        <v>45413</v>
-      </c>
+      <c r="J94" s="69"/>
       <c r="K94" s="71">
-        <v>46507</v>
+        <v>44895</v>
       </c>
       <c r="L94" s="73">
-        <v>383000</v>
+        <v>390000</v>
       </c>
       <c r="M94" s="6">
         <v>70000</v>
       </c>
       <c r="N94" s="20"/>
     </row>
-    <row r="95" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="29">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B95" s="29" t="s">
         <v>175</v>
@@ -7155,40 +7159,40 @@
         <v>9</v>
       </c>
       <c r="D95" s="58" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="E95" s="57" t="s">
         <v>173</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>182</v>
+        <v>129</v>
       </c>
       <c r="G95" s="59" t="s">
-        <v>65</v>
+        <v>176</v>
       </c>
       <c r="H95" s="62">
-        <v>137.52000000000001</v>
+        <v>1234.75</v>
       </c>
       <c r="I95" s="67" t="s">
         <v>3</v>
       </c>
       <c r="J95" s="69">
-        <v>43717</v>
+        <v>45200</v>
       </c>
       <c r="K95" s="71">
-        <v>45565</v>
+        <v>49308</v>
       </c>
       <c r="L95" s="73">
-        <v>0</v>
+        <v>367500</v>
       </c>
       <c r="M95" s="6">
         <v>70000</v>
       </c>
       <c r="N95" s="20"/>
     </row>
-    <row r="96" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="29">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B96" s="29" t="s">
         <v>175</v>
@@ -7197,7 +7201,7 @@
         <v>9</v>
       </c>
       <c r="D96" s="58" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="E96" s="57" t="s">
         <v>173</v>
@@ -7206,33 +7210,25 @@
         <v>182</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="H96" s="62">
-        <v>137.52000000000001</v>
+        <v>1234.75</v>
       </c>
       <c r="I96" s="67" t="s">
         <v>3</v>
       </c>
       <c r="J96" s="69">
-        <v>45566</v>
-      </c>
-      <c r="K96" s="71">
-        <v>49217</v>
-      </c>
-      <c r="L96" s="73">
-        <v>0</v>
-      </c>
-      <c r="M96" s="6">
-        <v>70000</v>
-      </c>
-      <c r="N96" s="20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>44896</v>
+      </c>
+      <c r="K96" s="71"/>
+      <c r="L96" s="73"/>
+      <c r="M96" s="6"/>
+      <c r="N96" s="20"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="29">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B97" s="29" t="s">
         <v>175</v>
@@ -7272,9 +7268,9 @@
       </c>
       <c r="N97" s="20"/>
     </row>
-    <row r="98" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="29">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B98" s="29" t="s">
         <v>175</v>
@@ -7314,9 +7310,9 @@
       </c>
       <c r="N98" s="20"/>
     </row>
-    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" s="29">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B99" s="29" t="s">
         <v>175</v>
@@ -7356,9 +7352,9 @@
       </c>
       <c r="N99" s="20"/>
     </row>
-    <row r="100" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="29">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B100" s="29" t="s">
         <v>175</v>
@@ -7396,7 +7392,7 @@
       </c>
       <c r="N100" s="20"/>
     </row>
-    <row r="101" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="29">
         <v>100</v>
       </c>
@@ -7407,7 +7403,7 @@
         <v>6</v>
       </c>
       <c r="D101" s="58" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="E101" s="57" t="s">
         <v>173</v>
@@ -7416,31 +7412,29 @@
         <v>182</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H101" s="62">
-        <v>548</v>
+        <v>938.59</v>
       </c>
       <c r="I101" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="J101" s="69">
-        <v>45962</v>
-      </c>
+      <c r="J101" s="69"/>
       <c r="K101" s="71">
-        <v>49248</v>
+        <v>45961</v>
       </c>
       <c r="L101" s="73">
-        <v>390000</v>
+        <v>410000</v>
       </c>
       <c r="M101" s="6">
         <v>70000</v>
       </c>
       <c r="N101" s="20"/>
     </row>
-    <row r="102" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="29">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B102" s="29" t="s">
         <v>175</v>
@@ -7449,7 +7443,7 @@
         <v>6</v>
       </c>
       <c r="D102" s="58" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="E102" s="57" t="s">
         <v>173</v>
@@ -7458,29 +7452,31 @@
         <v>182</v>
       </c>
       <c r="G102" s="59" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H102" s="62">
-        <v>938.59</v>
+        <v>548</v>
       </c>
       <c r="I102" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="J102" s="69"/>
+      <c r="J102" s="69">
+        <v>45962</v>
+      </c>
       <c r="K102" s="71">
-        <v>45961</v>
+        <v>49248</v>
       </c>
       <c r="L102" s="73">
-        <v>410000</v>
+        <v>390000</v>
       </c>
       <c r="M102" s="6">
         <v>70000</v>
       </c>
       <c r="N102" s="20"/>
     </row>
-    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="29">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B103" s="29" t="s">
         <v>175</v>
@@ -7520,9 +7516,9 @@
       </c>
       <c r="N103" s="20"/>
     </row>
-    <row r="104" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="29">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B104" s="29" t="s">
         <v>175</v>
@@ -7560,9 +7556,9 @@
       </c>
       <c r="N104" s="20"/>
     </row>
-    <row r="105" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="29">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B105" s="29" t="s">
         <v>175</v>
@@ -7602,9 +7598,9 @@
       </c>
       <c r="N105" s="20"/>
     </row>
-    <row r="106" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="29">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B106" s="29" t="s">
         <v>175</v>
@@ -7642,9 +7638,9 @@
       </c>
       <c r="N106" s="20"/>
     </row>
-    <row r="107" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="29">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B107" s="29" t="s">
         <v>175</v>
@@ -7684,9 +7680,9 @@
       </c>
       <c r="N107" s="20"/>
     </row>
-    <row r="108" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" s="29">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B108" s="29" t="s">
         <v>175</v>
@@ -7720,9 +7716,9 @@
       <c r="M108" s="14"/>
       <c r="N108" s="20"/>
     </row>
-    <row r="109" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" s="29">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B109" s="29" t="s">
         <v>175</v>
@@ -7756,9 +7752,9 @@
       <c r="M109" s="14"/>
       <c r="N109" s="20"/>
     </row>
-    <row r="110" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" s="29">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B110" s="29" t="s">
         <v>175</v>
@@ -7798,9 +7794,9 @@
       </c>
       <c r="N110" s="20"/>
     </row>
-    <row r="111" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" s="29">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B111" s="29" t="s">
         <v>175</v>
@@ -7840,9 +7836,9 @@
       </c>
       <c r="N111" s="20"/>
     </row>
-    <row r="112" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" s="29">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B112" s="29" t="s">
         <v>175</v>
@@ -7882,9 +7878,9 @@
       </c>
       <c r="N112" s="20"/>
     </row>
-    <row r="113" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="29">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B113" s="29" t="s">
         <v>175</v>
@@ -7924,9 +7920,9 @@
       </c>
       <c r="N113" s="20"/>
     </row>
-    <row r="114" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="29">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B114" s="29" t="s">
         <v>175</v>
@@ -7966,9 +7962,9 @@
       </c>
       <c r="N114" s="20"/>
     </row>
-    <row r="115" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="29">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B115" s="29" t="s">
         <v>175</v>
@@ -8008,9 +8004,9 @@
       </c>
       <c r="N115" s="20"/>
     </row>
-    <row r="116" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" s="29">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B116" s="29" t="s">
         <v>175</v>
@@ -8050,9 +8046,9 @@
       </c>
       <c r="N116" s="20"/>
     </row>
-    <row r="117" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" s="29">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B117" s="29" t="s">
         <v>175</v>
@@ -8092,9 +8088,9 @@
       </c>
       <c r="N117" s="20"/>
     </row>
-    <row r="118" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="29">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B118" s="29" t="s">
         <v>175</v>
@@ -8134,9 +8130,9 @@
       </c>
       <c r="N118" s="20"/>
     </row>
-    <row r="119" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" s="29">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B119" s="29" t="s">
         <v>175</v>
@@ -8170,9 +8166,9 @@
       <c r="M119" s="14"/>
       <c r="N119" s="20"/>
     </row>
-    <row r="120" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="29">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B120" s="29" t="s">
         <v>175</v>
@@ -8206,9 +8202,9 @@
       <c r="M120" s="14"/>
       <c r="N120" s="20"/>
     </row>
-    <row r="121" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="29">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B121" s="29" t="s">
         <v>175</v>
@@ -8242,9 +8238,9 @@
       <c r="M121" s="15"/>
       <c r="N121" s="20"/>
     </row>
-    <row r="122" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" s="29">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B122" s="29" t="s">
         <v>175</v>
@@ -8284,9 +8280,9 @@
       </c>
       <c r="N122" s="20"/>
     </row>
-    <row r="123" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" s="29">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B123" s="29" t="s">
         <v>175</v>
@@ -8326,9 +8322,9 @@
       </c>
       <c r="N123" s="20"/>
     </row>
-    <row r="124" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" s="29">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B124" s="29" t="s">
         <v>175</v>
@@ -8368,9 +8364,9 @@
       </c>
       <c r="N124" s="20"/>
     </row>
-    <row r="125" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" s="29">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B125" s="29" t="s">
         <v>175</v>
@@ -8410,9 +8406,9 @@
       </c>
       <c r="N125" s="20"/>
     </row>
-    <row r="126" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" s="29">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B126" s="29" t="s">
         <v>175</v>
@@ -8452,9 +8448,9 @@
       </c>
       <c r="N126" s="20"/>
     </row>
-    <row r="127" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="29">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B127" s="29" t="s">
         <v>175</v>
@@ -8486,9 +8482,9 @@
       <c r="M127" s="14"/>
       <c r="N127" s="20"/>
     </row>
-    <row r="128" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" s="29">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B128" s="29" t="s">
         <v>175</v>
@@ -8526,9 +8522,9 @@
       </c>
       <c r="N128" s="20"/>
     </row>
-    <row r="129" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" s="29">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B129" s="29" t="s">
         <v>175</v>
@@ -8566,9 +8562,9 @@
       </c>
       <c r="N129" s="20"/>
     </row>
-    <row r="130" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" s="29">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B130" s="29" t="s">
         <v>175</v>
@@ -8606,9 +8602,9 @@
       </c>
       <c r="N130" s="20"/>
     </row>
-    <row r="131" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" s="29">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B131" s="29" t="s">
         <v>175</v>
@@ -8648,9 +8644,9 @@
       </c>
       <c r="N131" s="20"/>
     </row>
-    <row r="132" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" s="29">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B132" s="29" t="s">
         <v>175</v>
@@ -8690,9 +8686,9 @@
       </c>
       <c r="N132" s="20"/>
     </row>
-    <row r="133" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" s="29">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B133" s="29" t="s">
         <v>175</v>
@@ -8730,9 +8726,9 @@
       <c r="M133" s="15"/>
       <c r="N133" s="20"/>
     </row>
-    <row r="134" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" s="29">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B134" s="29" t="s">
         <v>175</v>
@@ -8770,9 +8766,9 @@
       <c r="M134" s="15"/>
       <c r="N134" s="20"/>
     </row>
-    <row r="135" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" s="29">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B135" s="29" t="s">
         <v>175</v>
@@ -8812,9 +8808,9 @@
       </c>
       <c r="N135" s="20"/>
     </row>
-    <row r="136" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" s="29">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B136" s="29" t="s">
         <v>175</v>
@@ -8854,9 +8850,9 @@
       </c>
       <c r="N136" s="20"/>
     </row>
-    <row r="137" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" s="29">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B137" s="29" t="s">
         <v>175</v>
@@ -8894,9 +8890,9 @@
       <c r="M137" s="15"/>
       <c r="N137" s="20"/>
     </row>
-    <row r="138" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" s="29">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B138" s="29" t="s">
         <v>175</v>
@@ -8934,9 +8930,9 @@
       <c r="M138" s="15"/>
       <c r="N138" s="20"/>
     </row>
-    <row r="139" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" s="29">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B139" s="29" t="s">
         <v>175</v>
@@ -8976,9 +8972,9 @@
       </c>
       <c r="N139" s="20"/>
     </row>
-    <row r="140" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" s="29">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B140" s="29" t="s">
         <v>175</v>
@@ -9018,9 +9014,9 @@
       </c>
       <c r="N140" s="20"/>
     </row>
-    <row r="141" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" s="29">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B141" s="29" t="s">
         <v>175</v>
@@ -9058,9 +9054,9 @@
       <c r="M141" s="15"/>
       <c r="N141" s="20"/>
     </row>
-    <row r="142" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" s="29">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B142" s="29" t="s">
         <v>175</v>
@@ -9098,9 +9094,9 @@
       <c r="M142" s="15"/>
       <c r="N142" s="20"/>
     </row>
-    <row r="143" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" s="29">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B143" s="29" t="s">
         <v>175</v>
@@ -9140,9 +9136,9 @@
       </c>
       <c r="N143" s="20"/>
     </row>
-    <row r="144" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" s="29">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B144" s="29" t="s">
         <v>175</v>
@@ -9182,9 +9178,9 @@
       </c>
       <c r="N144" s="20"/>
     </row>
-    <row r="145" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" s="29">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B145" s="29" t="s">
         <v>175</v>
@@ -9216,9 +9212,9 @@
       </c>
       <c r="N145" s="20"/>
     </row>
-    <row r="146" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" s="29">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B146" s="29" t="s">
         <v>175</v>
@@ -9258,9 +9254,9 @@
       </c>
       <c r="N146" s="20"/>
     </row>
-    <row r="147" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" s="29">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B147" s="29" t="s">
         <v>175</v>
@@ -9298,9 +9294,9 @@
       <c r="M147" s="15"/>
       <c r="N147" s="20"/>
     </row>
-    <row r="148" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148" s="29">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B148" s="29" t="s">
         <v>175</v>
@@ -9338,9 +9334,9 @@
       <c r="M148" s="14"/>
       <c r="N148" s="20"/>
     </row>
-    <row r="149" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" s="29">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B149" s="29" t="s">
         <v>175</v>
@@ -9378,9 +9374,9 @@
       <c r="M149" s="14"/>
       <c r="N149" s="20"/>
     </row>
-    <row r="150" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" s="29">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B150" s="29" t="s">
         <v>175</v>
@@ -9414,9 +9410,9 @@
       <c r="M150" s="15"/>
       <c r="N150" s="20"/>
     </row>
-    <row r="151" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" s="29">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B151" s="29" t="s">
         <v>175</v>
@@ -9450,9 +9446,9 @@
       <c r="M151" s="15"/>
       <c r="N151" s="20"/>
     </row>
-    <row r="152" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152" s="29">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B152" s="29" t="s">
         <v>175</v>
@@ -9486,9 +9482,9 @@
       <c r="M152" s="15"/>
       <c r="N152" s="20"/>
     </row>
-    <row r="153" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" s="29">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B153" s="29" t="s">
         <v>175</v>
@@ -9522,9 +9518,9 @@
       <c r="M153" s="15"/>
       <c r="N153" s="20"/>
     </row>
-    <row r="154" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" s="29">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B154" s="29" t="s">
         <v>175</v>
@@ -9558,9 +9554,9 @@
       <c r="M154" s="15"/>
       <c r="N154" s="20"/>
     </row>
-    <row r="155" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" s="29">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B155" s="29" t="s">
         <v>175</v>
@@ -9594,9 +9590,9 @@
       <c r="M155" s="15"/>
       <c r="N155" s="20"/>
     </row>
-    <row r="156" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" s="29">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B156" s="29" t="s">
         <v>175</v>
@@ -9634,9 +9630,9 @@
       <c r="M156" s="15"/>
       <c r="N156" s="20"/>
     </row>
-    <row r="157" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" s="29">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B157" s="29" t="s">
         <v>175</v>
@@ -9676,9 +9672,9 @@
       </c>
       <c r="N157" s="20"/>
     </row>
-    <row r="158" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" s="29">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B158" s="29" t="s">
         <v>175</v>
@@ -9718,9 +9714,9 @@
       </c>
       <c r="N158" s="20"/>
     </row>
-    <row r="159" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" s="29">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B159" s="29" t="s">
         <v>175</v>

</xml_diff>